<commit_message>
arreglos bidimensionales, multiplicacion de matrices, mayor y menor
</commit_message>
<xml_diff>
--- a/Libro1.xlsx
+++ b/Libro1.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://alumnoudg-my.sharepoint.com/personal/jluis_lopezg_alumno_udg_mx/Documents/DIFERENTE/POO-y-C/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E0456471-F11B-413C-AC21-6031D3E156C6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="10" documentId="8_{E0456471-F11B-413C-AC21-6031D3E156C6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{42DB47DF-91A3-4CEF-8F42-FE3912654D44}"/>
   <bookViews>
-    <workbookView xWindow="3510" yWindow="3510" windowWidth="21600" windowHeight="11385" xr2:uid="{03B7E412-C7BA-4628-B73A-CB71A268FC2C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{03B7E412-C7BA-4628-B73A-CB71A268FC2C}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -399,7 +400,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B2F12D4-7A62-45BE-A90D-27C0B5B54DD5}">
   <dimension ref="B2:E8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
@@ -506,4 +507,82 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C699BB67-16AA-40F7-8A44-918BE6615919}">
+  <dimension ref="C3:K5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="3" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C3">
+        <v>3</v>
+      </c>
+      <c r="D3">
+        <v>4</v>
+      </c>
+      <c r="E3">
+        <v>5</v>
+      </c>
+      <c r="G3">
+        <v>3</v>
+      </c>
+      <c r="H3">
+        <v>4</v>
+      </c>
+      <c r="I3">
+        <v>5</v>
+      </c>
+      <c r="K3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C4">
+        <v>3</v>
+      </c>
+      <c r="D4">
+        <v>4</v>
+      </c>
+      <c r="E4">
+        <v>5</v>
+      </c>
+      <c r="G4">
+        <v>3</v>
+      </c>
+      <c r="H4">
+        <v>4</v>
+      </c>
+      <c r="I4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C5">
+        <v>3</v>
+      </c>
+      <c r="D5">
+        <v>4</v>
+      </c>
+      <c r="E5">
+        <v>5</v>
+      </c>
+      <c r="G5">
+        <v>3</v>
+      </c>
+      <c r="H5">
+        <v>4</v>
+      </c>
+      <c r="I5">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>